<commit_message>
-> Re-run DPLKINV023-001 (Setup Custodian) -> Scripting DPLKINV142-001 until DPLKINV143-001, DPLKINV151-001, and DPLKINV151-002 (Deposito Penerimaan) -> Scripting DPLKINV147-001 until DPLKINV150-002 (Deposito Jatuh Tempo) -> Scripting DPLKINV162-001 until DPLKINV163-002 (Pembatalan Redemption)
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV023-001 Until DPLKINV023-003 - Setup Custodian Investasi - Approve Data.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV023-001 Until DPLKINV023-003 - Setup Custodian Investasi - Approve Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E849C75-2ED1-4964-9F95-0B73458EEDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91033F3-2E3C-43E4-9C8F-346E02D39610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -784,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA6C01D8-A243-4074-80A9-65DC8902E8C8}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,7 +854,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>